<commit_message>
started editing mainboard FM
</commit_message>
<xml_diff>
--- a/hardware/foras-promineo-EM/fabrication-data/mainboard_log.xlsx
+++ b/hardware/foras-promineo-EM/fabrication-data/mainboard_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GitHub\mainboard\hardware\foras-promineo-proto\fabrication-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GitHub\mainboard\hardware\foras-promineo-EM\fabrication-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D1E8B-C7BC-44EA-A718-E5689C858C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7876185-539A-4204-84DF-FC8333027619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Action</t>
   </si>
@@ -151,6 +151,36 @@
   </si>
   <si>
     <t>buy rf connectors</t>
+  </si>
+  <si>
+    <t>added ground GPS and LoRa units</t>
+  </si>
+  <si>
+    <t>USB Battery charger IC is wrong P/N, needs changed</t>
+  </si>
+  <si>
+    <t>5V_debug current draw when idle = 82mA</t>
+  </si>
+  <si>
+    <t>V_RF and V_PYLD measured at 5.04V @ no load</t>
+  </si>
+  <si>
+    <t>verified comms I2C devices(besides USB battery charger)</t>
+  </si>
+  <si>
+    <t>3/?/21</t>
+  </si>
+  <si>
+    <t>firmware loaded successfully</t>
+  </si>
+  <si>
+    <t>board runs basic_eval program, not all systems interfaced but no noticeable errors found.</t>
+  </si>
+  <si>
+    <t>7V applied to VBATT +/-'s and idle draw was 22mA, V_RF and V_PYLD at 5.04V</t>
+  </si>
+  <si>
+    <t>daignosing issue with solar charge regulator</t>
   </si>
 </sst>
 </file>
@@ -257,10 +287,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,8 +566,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FEFF7DE-A67C-4C3A-A9CC-F9E3800B285E}" name="Table13" displayName="Table13" ref="A2:C9" totalsRowShown="0">
-  <autoFilter ref="A2:C9" xr:uid="{1FEFF7DE-A67C-4C3A-A9CC-F9E3800B285E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FEFF7DE-A67C-4C3A-A9CC-F9E3800B285E}" name="Table13" displayName="Table13" ref="A2:C18" totalsRowShown="0">
+  <autoFilter ref="A2:C18" xr:uid="{1FEFF7DE-A67C-4C3A-A9CC-F9E3800B285E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{466C48AE-01DC-404F-A009-2DC876DB47D5}" name="Date" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{892E8C3D-61AE-4500-B3BB-B6E801783EEB}" name="Action" dataDxfId="1"/>
@@ -1683,10 +1713,10 @@
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1900,16 +1930,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0D637E-8E83-4439-8ECA-4CBE01750993}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
@@ -1920,10 +1950,10 @@
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1987,7 +2017,7 @@
       <c r="A6" s="5">
         <v>44254</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1995,7 +2025,7 @@
       <c r="A7" s="5">
         <v>44254</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2003,7 +2033,7 @@
       <c r="A8" s="5">
         <v>44254</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2011,8 +2041,80 @@
       <c r="A9" s="5">
         <v>44254</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>44268</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>44268</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>44269</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>44269</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>44270</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>44270</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>44270</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>44270</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>